<commit_message>
Major Update - Added 2021
Added 2021 report and updated version of 2020 report. 2020 had to be reduced in size to fit under the 100MB file size limit for GitHub. I did this by replacing 16 bit png files with 8 bit jpg files reduced to half size.
</commit_message>
<xml_diff>
--- a/SS-OBS-DB.xlsx
+++ b/SS-OBS-DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Astronomy\Projects\GeneralDocumentation\ObservingReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B525063-7C6A-4FC8-99EF-5311A4D36180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517F584E-2CE7-4B42-B566-2E41353A4844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="-110" windowWidth="18020" windowHeight="11020" tabRatio="700" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29910" yWindow="1395" windowWidth="16575" windowHeight="13500" tabRatio="700" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="8" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="835">
   <si>
     <r>
       <t>Imaging</t>
@@ -8325,7 +8325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="268">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -9081,6 +9081,9 @@
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="12" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13571,9 +13574,8 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
+              <a:schemeClr val="accent1">
+                <a:alpha val="25000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -13585,10 +13587,10 @@
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Mars!$F$114:$F$117</c:f>
+              <c:f>Mars!$F$114:$F$147</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>237</c:v>
                 </c:pt>
@@ -13600,16 +13602,64 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Mars!$G$114:$G$117</c:f>
+              <c:f>Mars!$G$114:$G$147</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>12.5</c:v>
                 </c:pt>
@@ -13621,16 +13671,64 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:bubbleSize>
             <c:numRef>
-              <c:f>Mars!$Y$114:$Y$117</c:f>
+              <c:f>Mars!$Y$114:$Y$147</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>0.85741203863731208</c:v>
                 </c:pt>
@@ -13642,6 +13740,54 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.2106205692696455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82940573544883622</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.330703483965108</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9413174399786064</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0680499733415203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1495119171773631</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4144257057082155</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1335007433937638</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6160954714877225</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3823441762017117</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4099838977082526</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4797541315657996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4346854778125266</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2844566319682831</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2694337473838584</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1632764504911628</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.086996406755921</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14839,9 +14985,8 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
+              <a:schemeClr val="accent1">
+                <a:alpha val="25000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -14853,10 +14998,10 @@
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Mars!$F$114:$F$117</c:f>
+              <c:f>Mars!$F$114:$F$147</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>237</c:v>
                 </c:pt>
@@ -14868,16 +15013,64 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Mars!$E$114:$E$117</c:f>
+              <c:f>Mars!$E$114:$E$147</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>117.8</c:v>
                 </c:pt>
@@ -14889,16 +15082,64 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>275.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>344.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>238.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>324.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>84.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>128.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>54.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>271.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>156.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>92.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:bubbleSize>
             <c:numRef>
-              <c:f>Mars!$Y$114:$Y$117</c:f>
+              <c:f>Mars!$Y$114:$Y$147</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>0.85741203863731208</c:v>
                 </c:pt>
@@ -14910,6 +15151,54 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.2106205692696455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82940573544883622</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.330703483965108</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9413174399786064</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0680499733415203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1495119171773631</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4144257057082155</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1335007433937638</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6160954714877225</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3823441762017117</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4099838977082526</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4797541315657996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4346854778125266</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2844566319682831</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2694337473838584</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1632764504911628</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.086996406755921</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16258,7 +16547,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16334,7 +16623,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654143" cy="6277429"/>
+    <xdr:ext cx="12981214" cy="9416143"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -35665,13 +35954,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA125"/>
+  <dimension ref="A1:AA133"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D102" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
-      <selection pane="bottomRight" activeCell="F113" sqref="F113"/>
+      <selection pane="bottomRight" activeCell="M133" sqref="M133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -44142,195 +44431,1155 @@
     </row>
     <row r="118" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="22"/>
-      <c r="C118" s="36"/>
-      <c r="D118" s="123"/>
-      <c r="E118" s="126"/>
-      <c r="F118" s="114"/>
-      <c r="G118" s="13"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="121"/>
+      <c r="C118" s="36">
+        <v>44076.25</v>
+      </c>
+      <c r="D118" s="123">
+        <v>0.08</v>
+      </c>
+      <c r="E118" s="126">
+        <v>275.39999999999998</v>
+      </c>
+      <c r="F118" s="114">
+        <v>270</v>
+      </c>
+      <c r="G118" s="13">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="H118" s="13">
+        <v>-1.8</v>
+      </c>
+      <c r="I118" s="13">
+        <f t="shared" ref="I118" si="154">-LOG((1/(G118^2))*(2.511^(-H118)))/LOG(2.511)</f>
+        <v>4.6076223538567387</v>
+      </c>
+      <c r="J118" s="121" t="s">
+        <v>435</v>
+      </c>
       <c r="K118" s="121"/>
       <c r="L118" s="121"/>
-      <c r="M118" s="13"/>
-      <c r="N118" s="143"/>
+      <c r="M118" s="13">
+        <v>27</v>
+      </c>
+      <c r="N118" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O118" s="5">
+        <v>0</v>
+      </c>
+      <c r="P118" s="5">
+        <v>1</v>
+      </c>
       <c r="Q118" s="22"/>
-      <c r="R118" s="6"/>
-      <c r="S118" s="62"/>
-      <c r="T118" s="6"/>
-      <c r="U118" s="114"/>
-      <c r="V118" s="114"/>
-      <c r="W118" s="26"/>
-      <c r="X118" s="26"/>
-      <c r="Y118" s="26"/>
+      <c r="R118" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S118" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T118" s="256">
+        <f t="shared" ref="T118" si="155">1/SIN(RADIANS(M118+244/(165+47*M118^1.1)))</f>
+        <v>2.1931939234339084</v>
+      </c>
+      <c r="U118" s="114">
+        <f t="shared" ref="U118" si="156">DEGREES(ASIN(SIN(RADIANS(F118))*SIN(RADIANS(25.19))))</f>
+        <v>-25.19</v>
+      </c>
+      <c r="V118" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W118" s="26">
+        <f t="shared" ref="W118" si="157">668.5921*MOD((C118-Z$1),686.9726)/686.9726</f>
+        <v>514.57779508928706</v>
+      </c>
+      <c r="X118" s="26">
+        <f t="shared" ref="X118" si="158">(S118/(G118/2))*T118/(IF(ISBLANK(N118),0.5,N118))</f>
+        <v>0.12056825233537191</v>
+      </c>
+      <c r="Y118" s="26">
+        <f t="shared" ref="Y118" si="159">0.1/X118</f>
+        <v>0.82940573544883622</v>
+      </c>
     </row>
     <row r="119" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="22"/>
-      <c r="C119" s="36"/>
-      <c r="D119" s="123"/>
-      <c r="E119" s="126"/>
-      <c r="F119" s="114"/>
-      <c r="G119" s="13"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="13"/>
-      <c r="J119" s="121"/>
+      <c r="C119" s="36">
+        <v>44078.5</v>
+      </c>
+      <c r="D119" s="123">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E119" s="126">
+        <v>344.7</v>
+      </c>
+      <c r="F119" s="114">
+        <v>272</v>
+      </c>
+      <c r="G119" s="13">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="H119" s="13">
+        <v>-1.9</v>
+      </c>
+      <c r="I119" s="13">
+        <f t="shared" ref="I119" si="160">-LOG((1/(G119^2))*(2.511^(-H119)))/LOG(2.511)</f>
+        <v>4.5414771410404358</v>
+      </c>
+      <c r="J119" s="121" t="s">
+        <v>435</v>
+      </c>
       <c r="K119" s="121"/>
       <c r="L119" s="121"/>
-      <c r="M119" s="13"/>
-      <c r="N119" s="143"/>
+      <c r="M119" s="13">
+        <v>46</v>
+      </c>
+      <c r="N119" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O119" s="5">
+        <v>0</v>
+      </c>
+      <c r="P119" s="5">
+        <v>1</v>
+      </c>
       <c r="Q119" s="22"/>
-      <c r="R119" s="6"/>
-      <c r="S119" s="62"/>
-      <c r="T119" s="6"/>
-      <c r="U119" s="114"/>
-      <c r="V119" s="114"/>
-      <c r="W119" s="26"/>
-      <c r="X119" s="26"/>
-      <c r="Y119" s="26"/>
+      <c r="R119" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S119" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T119" s="256">
+        <f t="shared" ref="T119" si="161">1/SIN(RADIANS(M119+244/(165+47*M119^1.1)))</f>
+        <v>1.3884528521062274</v>
+      </c>
+      <c r="U119" s="114">
+        <f t="shared" ref="U119" si="162">DEGREES(ASIN(SIN(RADIANS(F119))*SIN(RADIANS(25.19))))</f>
+        <v>-25.173584421552981</v>
+      </c>
+      <c r="V119" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W119" s="26">
+        <f t="shared" ref="W119" si="163">668.5921*MOD((C119-Z$1),686.9726)/686.9726</f>
+        <v>516.76759454417061</v>
+      </c>
+      <c r="X119" s="26">
+        <f t="shared" ref="X119" si="164">(S119/(G119/2))*T119/(IF(ISBLANK(N119),0.5,N119))</f>
+        <v>7.5148221376883442E-2</v>
+      </c>
+      <c r="Y119" s="26">
+        <f t="shared" ref="Y119" si="165">0.1/X119</f>
+        <v>1.330703483965108</v>
+      </c>
     </row>
     <row r="120" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="22"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="123"/>
-      <c r="E120" s="126"/>
-      <c r="F120" s="114"/>
-      <c r="G120" s="13"/>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
-      <c r="J120" s="121"/>
+      <c r="C120" s="36">
+        <v>44080.25</v>
+      </c>
+      <c r="D120" s="123">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E120" s="126">
+        <v>238.7</v>
+      </c>
+      <c r="F120" s="114">
+        <v>273</v>
+      </c>
+      <c r="G120" s="13">
+        <v>19.7</v>
+      </c>
+      <c r="H120" s="13">
+        <v>-1.9</v>
+      </c>
+      <c r="I120" s="13">
+        <f t="shared" ref="I120" si="166">-LOG((1/(G120^2))*(2.511^(-H120)))/LOG(2.511)</f>
+        <v>4.5748123968745968</v>
+      </c>
+      <c r="J120" s="121" t="s">
+        <v>435</v>
+      </c>
       <c r="K120" s="121"/>
       <c r="L120" s="121"/>
-      <c r="M120" s="13"/>
-      <c r="N120" s="143"/>
+      <c r="M120" s="13">
+        <v>30</v>
+      </c>
+      <c r="N120" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O120" s="5">
+        <v>0</v>
+      </c>
+      <c r="P120" s="5">
+        <v>1</v>
+      </c>
       <c r="Q120" s="22"/>
-      <c r="R120" s="6"/>
-      <c r="S120" s="62"/>
-      <c r="T120" s="6"/>
-      <c r="U120" s="114"/>
-      <c r="V120" s="114"/>
-      <c r="W120" s="26"/>
-      <c r="X120" s="26"/>
-      <c r="Y120" s="26"/>
+      <c r="R120" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S120" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T120" s="256">
+        <f t="shared" ref="T120" si="167">1/SIN(RADIANS(M120+244/(165+47*M120^1.1)))</f>
+        <v>1.9931538464145713</v>
+      </c>
+      <c r="U120" s="114">
+        <f t="shared" ref="U120" si="168">DEGREES(ASIN(SIN(RADIANS(F120))*SIN(RADIANS(25.19))))</f>
+        <v>-25.15307274301146</v>
+      </c>
+      <c r="V120" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W120" s="26">
+        <f t="shared" ref="W120" si="169">668.5921*MOD((C120-Z$1),686.9726)/686.9726</f>
+        <v>518.47077189796903</v>
+      </c>
+      <c r="X120" s="26">
+        <f t="shared" ref="X120" si="170">(S120/(G120/2))*T120/(IF(ISBLANK(N120),0.5,N120))</f>
+        <v>0.1062340882606751</v>
+      </c>
+      <c r="Y120" s="26">
+        <f t="shared" ref="Y120" si="171">0.1/X120</f>
+        <v>0.9413174399786064</v>
+      </c>
     </row>
     <row r="121" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="22"/>
-      <c r="C121" s="36"/>
-      <c r="D121" s="123"/>
-      <c r="E121" s="126"/>
-      <c r="F121" s="114"/>
-      <c r="G121" s="13"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="13"/>
-      <c r="J121" s="121"/>
+      <c r="C121" s="36">
+        <v>44090.229166666664</v>
+      </c>
+      <c r="D121" s="123">
+        <v>0.04</v>
+      </c>
+      <c r="E121" s="126">
+        <v>140.5</v>
+      </c>
+      <c r="F121" s="114">
+        <v>279</v>
+      </c>
+      <c r="G121" s="13">
+        <v>21.1</v>
+      </c>
+      <c r="H121" s="13">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="I121" s="13">
+        <f t="shared" ref="I121" si="172">-LOG((1/(G121^2))*(2.511^(-H121)))/LOG(2.511)</f>
+        <v>4.4239506950679193</v>
+      </c>
+      <c r="J121" s="121" t="s">
+        <v>435</v>
+      </c>
       <c r="K121" s="121"/>
       <c r="L121" s="121"/>
-      <c r="M121" s="13"/>
-      <c r="N121" s="143"/>
+      <c r="M121" s="13">
+        <v>32</v>
+      </c>
+      <c r="N121" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O121" s="5">
+        <v>0</v>
+      </c>
+      <c r="P121" s="5">
+        <v>1</v>
+      </c>
       <c r="Q121" s="22"/>
-      <c r="R121" s="6"/>
-      <c r="S121" s="62"/>
-      <c r="T121" s="6"/>
-      <c r="U121" s="114"/>
-      <c r="V121" s="114"/>
-      <c r="W121" s="26"/>
-      <c r="X121" s="26"/>
-      <c r="Y121" s="26"/>
+      <c r="R121" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S121" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T121" s="256">
+        <f t="shared" ref="T121" si="173">1/SIN(RADIANS(M121+244/(165+47*M121^1.1)))</f>
+        <v>1.8814885629712417</v>
+      </c>
+      <c r="U121" s="114">
+        <f t="shared" ref="U121" si="174">DEGREES(ASIN(SIN(RADIANS(F121))*SIN(RADIANS(25.19))))</f>
+        <v>-24.858660219368051</v>
+      </c>
+      <c r="V121" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W121" s="26">
+        <f t="shared" ref="W121" si="175">668.5921*MOD((C121-Z$1),686.9726)/686.9726</f>
+        <v>528.18293799879325</v>
+      </c>
+      <c r="X121" s="26">
+        <f t="shared" ref="X121" si="176">(S121/(G121/2))*T121/(IF(ISBLANK(N121),0.5,N121))</f>
+        <v>9.3628577778189739E-2</v>
+      </c>
+      <c r="Y121" s="26">
+        <f t="shared" ref="Y121" si="177">0.1/X121</f>
+        <v>1.0680499733415203</v>
+      </c>
     </row>
     <row r="122" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="22"/>
-      <c r="C122" s="36"/>
-      <c r="D122" s="123"/>
-      <c r="E122" s="126"/>
-      <c r="F122" s="114"/>
-      <c r="G122" s="13"/>
-      <c r="H122" s="13"/>
-      <c r="I122" s="13"/>
-      <c r="J122" s="121"/>
+      <c r="C122" s="36">
+        <v>44099.208333333336</v>
+      </c>
+      <c r="D122" s="123">
+        <v>0.02</v>
+      </c>
+      <c r="E122" s="126">
+        <v>52.6</v>
+      </c>
+      <c r="F122" s="114">
+        <v>284</v>
+      </c>
+      <c r="G122" s="13">
+        <v>22.1</v>
+      </c>
+      <c r="H122" s="13">
+        <v>-2.4</v>
+      </c>
+      <c r="I122" s="13">
+        <f t="shared" ref="I122" si="178">-LOG((1/(G122^2))*(2.511^(-H122)))/LOG(2.511)</f>
+        <v>4.3245383340207315</v>
+      </c>
+      <c r="J122" s="121" t="s">
+        <v>435</v>
+      </c>
       <c r="K122" s="121"/>
       <c r="L122" s="121"/>
-      <c r="M122" s="13"/>
-      <c r="N122" s="143"/>
+      <c r="M122" s="13">
+        <v>33</v>
+      </c>
+      <c r="N122" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O122" s="5">
+        <v>0</v>
+      </c>
+      <c r="P122" s="5">
+        <v>1</v>
+      </c>
       <c r="Q122" s="22"/>
-      <c r="R122" s="6"/>
-      <c r="S122" s="62"/>
-      <c r="T122" s="6"/>
-      <c r="U122" s="114"/>
-      <c r="V122" s="114"/>
-      <c r="W122" s="26"/>
-      <c r="X122" s="26"/>
-      <c r="Y122" s="26"/>
+      <c r="R122" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S122" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T122" s="256">
+        <f t="shared" ref="T122" si="179">1/SIN(RADIANS(M122+244/(165+47*M122^1.1)))</f>
+        <v>1.8310048580706904</v>
+      </c>
+      <c r="U122" s="114">
+        <f t="shared" ref="U122" si="180">DEGREES(ASIN(SIN(RADIANS(F122))*SIN(RADIANS(25.19))))</f>
+        <v>-24.392082987923679</v>
+      </c>
+      <c r="V122" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W122" s="26">
+        <f t="shared" ref="W122" si="181">668.5921*MOD((C122-Z$1),686.9726)/686.9726</f>
+        <v>536.92185989745394</v>
+      </c>
+      <c r="X122" s="26">
+        <f t="shared" ref="X122" si="182">(S122/(G122/2))*T122/(IF(ISBLANK(N122),0.5,N122))</f>
+        <v>8.6993443482996591E-2</v>
+      </c>
+      <c r="Y122" s="26">
+        <f t="shared" ref="Y122" si="183">0.1/X122</f>
+        <v>1.1495119171773631</v>
+      </c>
     </row>
     <row r="123" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="22"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="123"/>
-      <c r="E123" s="126"/>
-      <c r="F123" s="114"/>
-      <c r="G123" s="13"/>
-      <c r="H123" s="13"/>
-      <c r="I123" s="13"/>
-      <c r="J123" s="121"/>
+      <c r="C123" s="36">
+        <v>44109.208333333336</v>
+      </c>
+      <c r="D123" s="123">
+        <v>0.01</v>
+      </c>
+      <c r="E123" s="126">
+        <v>324.10000000000002</v>
+      </c>
+      <c r="F123" s="114">
+        <v>291</v>
+      </c>
+      <c r="G123" s="13">
+        <v>22.6</v>
+      </c>
+      <c r="H123" s="13">
+        <v>-2.4</v>
+      </c>
+      <c r="I123" s="13">
+        <f t="shared" ref="I123" si="184">-LOG((1/(G123^2))*(2.511^(-H123)))/LOG(2.511)</f>
+        <v>4.3731377855273701</v>
+      </c>
+      <c r="J123" s="121" t="s">
+        <v>435</v>
+      </c>
       <c r="K123" s="121"/>
       <c r="L123" s="121"/>
-      <c r="M123" s="13"/>
-      <c r="N123" s="143"/>
+      <c r="M123" s="13">
+        <v>41</v>
+      </c>
+      <c r="N123" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O123" s="5">
+        <v>0</v>
+      </c>
+      <c r="P123" s="5">
+        <v>1</v>
+      </c>
       <c r="Q123" s="22"/>
-      <c r="R123" s="6"/>
-      <c r="S123" s="62"/>
-      <c r="T123" s="6"/>
-      <c r="U123" s="114"/>
-      <c r="V123" s="114"/>
-      <c r="W123" s="26"/>
-      <c r="X123" s="26"/>
-      <c r="Y123" s="26"/>
+      <c r="R123" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S123" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T123" s="256">
+        <f t="shared" ref="T123" si="185">1/SIN(RADIANS(M123+244/(165+47*M123^1.1)))</f>
+        <v>1.5217348947311704</v>
+      </c>
+      <c r="U123" s="114">
+        <f t="shared" ref="U123" si="186">DEGREES(ASIN(SIN(RADIANS(F123))*SIN(RADIANS(25.19))))</f>
+        <v>-23.41272910300189</v>
+      </c>
+      <c r="V123" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W123" s="26">
+        <f t="shared" ref="W123" si="187">668.5921*MOD((C123-Z$1),686.9726)/686.9726</f>
+        <v>546.65430191915914</v>
+      </c>
+      <c r="X123" s="26">
+        <f t="shared" ref="X123" si="188">(S123/(G123/2))*T123/(IF(ISBLANK(N123),0.5,N123))</f>
+        <v>7.0700072542819861E-2</v>
+      </c>
+      <c r="Y123" s="26">
+        <f t="shared" ref="Y123" si="189">0.1/X123</f>
+        <v>1.4144257057082155</v>
+      </c>
     </row>
     <row r="124" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B124" s="22"/>
-      <c r="C124" s="36"/>
-      <c r="D124" s="123"/>
-      <c r="E124" s="126"/>
-      <c r="F124" s="114"/>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="13"/>
-      <c r="J124" s="121"/>
+      <c r="C124" s="36">
+        <v>44132.104166666664</v>
+      </c>
+      <c r="D124" s="123">
+        <v>0.01</v>
+      </c>
+      <c r="E124" s="126">
+        <v>84.7</v>
+      </c>
+      <c r="F124" s="114">
+        <v>304</v>
+      </c>
+      <c r="G124" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="H124" s="13">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="I124" s="13">
+        <f t="shared" ref="I124" si="190">-LOG((1/(G124^2))*(2.511^(-H124)))/LOG(2.511)</f>
+        <v>4.2823742129986879</v>
+      </c>
+      <c r="J124" s="121" t="s">
+        <v>435</v>
+      </c>
       <c r="K124" s="121"/>
       <c r="L124" s="121"/>
-      <c r="M124" s="13"/>
-      <c r="N124" s="143"/>
+      <c r="M124" s="13">
+        <v>35</v>
+      </c>
+      <c r="N124" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O124" s="5">
+        <v>0</v>
+      </c>
+      <c r="P124" s="5">
+        <v>1</v>
+      </c>
       <c r="Q124" s="22"/>
-      <c r="R124" s="6"/>
-      <c r="S124" s="62"/>
-      <c r="T124" s="6"/>
-      <c r="U124" s="114"/>
-      <c r="V124" s="114"/>
-      <c r="W124" s="26"/>
-      <c r="X124" s="26"/>
-      <c r="Y124" s="26"/>
+      <c r="R124" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S124" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T124" s="256">
+        <f t="shared" ref="T124" si="191">1/SIN(RADIANS(M124+244/(165+47*M124^1.1)))</f>
+        <v>1.7392388870659281</v>
+      </c>
+      <c r="U124" s="114">
+        <f t="shared" ref="U124" si="192">DEGREES(ASIN(SIN(RADIANS(F124))*SIN(RADIANS(25.19))))</f>
+        <v>-20.662106883307455</v>
+      </c>
+      <c r="V124" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W124" s="26">
+        <f t="shared" ref="W124" si="193">668.5921*MOD((C124-Z$1),686.9726)/686.9726</f>
+        <v>568.93753896468331</v>
+      </c>
+      <c r="X124" s="26">
+        <f t="shared" ref="X124" si="194">(S124/(G124/2))*T124/(IF(ISBLANK(N124),0.5,N124))</f>
+        <v>8.8222262387402134E-2</v>
+      </c>
+      <c r="Y124" s="26">
+        <f t="shared" ref="Y124" si="195">0.1/X124</f>
+        <v>1.1335007433937638</v>
+      </c>
     </row>
     <row r="125" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="22"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="123"/>
-      <c r="E125" s="126"/>
-      <c r="F125" s="114"/>
-      <c r="G125" s="13"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
-      <c r="J125" s="121"/>
+      <c r="C125" s="36">
+        <v>44132.229166666664</v>
+      </c>
+      <c r="D125" s="123">
+        <v>0.01</v>
+      </c>
+      <c r="E125" s="126">
+        <v>128.5</v>
+      </c>
+      <c r="F125" s="114">
+        <v>304</v>
+      </c>
+      <c r="G125" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="H125" s="13">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="I125" s="13">
+        <f t="shared" ref="I125" si="196">-LOG((1/(G125^2))*(2.511^(-H125)))/LOG(2.511)</f>
+        <v>4.2823742129986879</v>
+      </c>
+      <c r="J125" s="121" t="s">
+        <v>435</v>
+      </c>
       <c r="K125" s="121"/>
       <c r="L125" s="121"/>
-      <c r="M125" s="13"/>
-      <c r="N125" s="143"/>
+      <c r="M125" s="13">
+        <v>55</v>
+      </c>
+      <c r="N125" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O125" s="5">
+        <v>0</v>
+      </c>
+      <c r="P125" s="5">
+        <v>1</v>
+      </c>
       <c r="Q125" s="22"/>
-      <c r="R125" s="6"/>
-      <c r="S125" s="62"/>
-      <c r="T125" s="6"/>
-      <c r="U125" s="114"/>
-      <c r="V125" s="114"/>
-      <c r="W125" s="26"/>
-      <c r="X125" s="26"/>
-      <c r="Y125" s="26"/>
+      <c r="R125" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S125" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T125" s="256">
+        <f t="shared" ref="T125" si="197">1/SIN(RADIANS(M125+244/(165+47*M125^1.1)))</f>
+        <v>1.2198713542670481</v>
+      </c>
+      <c r="U125" s="114">
+        <f t="shared" ref="U125" si="198">DEGREES(ASIN(SIN(RADIANS(F125))*SIN(RADIANS(25.19))))</f>
+        <v>-20.662106883307455</v>
+      </c>
+      <c r="V125" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W125" s="26">
+        <f t="shared" ref="W125" si="199">668.5921*MOD((C125-Z$1),686.9726)/686.9726</f>
+        <v>569.05919448995462</v>
+      </c>
+      <c r="X125" s="26">
+        <f t="shared" ref="X125" si="200">(S125/(G125/2))*T125/(IF(ISBLANK(N125),0.5,N125))</f>
+        <v>6.1877532462821273E-2</v>
+      </c>
+      <c r="Y125" s="26">
+        <f t="shared" ref="Y125" si="201">0.1/X125</f>
+        <v>1.6160954714877225</v>
+      </c>
+    </row>
+    <row r="126" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="22"/>
+      <c r="C126" s="36">
+        <v>44133.145833333336</v>
+      </c>
+      <c r="D126" s="123">
+        <v>0.01</v>
+      </c>
+      <c r="E126" s="126">
+        <v>90.4</v>
+      </c>
+      <c r="F126" s="114">
+        <v>305</v>
+      </c>
+      <c r="G126" s="13">
+        <v>20.5</v>
+      </c>
+      <c r="H126" s="13">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="I126" s="13">
+        <f t="shared" ref="I126" si="202">-LOG((1/(G126^2))*(2.511^(-H126)))/LOG(2.511)</f>
+        <v>4.3612837087274139</v>
+      </c>
+      <c r="J126" s="121" t="s">
+        <v>435</v>
+      </c>
+      <c r="K126" s="121"/>
+      <c r="L126" s="121"/>
+      <c r="M126" s="13">
+        <v>45</v>
+      </c>
+      <c r="N126" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O126" s="5">
+        <v>0</v>
+      </c>
+      <c r="P126" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q126" s="22"/>
+      <c r="R126" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S126" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T126" s="256">
+        <f t="shared" ref="T126" si="203">1/SIN(RADIANS(M126+244/(165+47*M126^1.1)))</f>
+        <v>1.4123696442557017</v>
+      </c>
+      <c r="U126" s="114">
+        <f t="shared" ref="U126" si="204">DEGREES(ASIN(SIN(RADIANS(F126))*SIN(RADIANS(25.19))))</f>
+        <v>-20.404680299322521</v>
+      </c>
+      <c r="V126" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W126" s="26">
+        <f t="shared" ref="W126" si="205">668.5921*MOD((C126-Z$1),686.9726)/686.9726</f>
+        <v>569.95133500861562</v>
+      </c>
+      <c r="X126" s="26">
+        <f t="shared" ref="X126" si="206">(S126/(G126/2))*T126/(IF(ISBLANK(N126),0.5,N126))</f>
+        <v>7.2340884217974966E-2</v>
+      </c>
+      <c r="Y126" s="26">
+        <f t="shared" ref="Y126" si="207">0.1/X126</f>
+        <v>1.3823441762017117</v>
+      </c>
+    </row>
+    <row r="127" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="22"/>
+      <c r="C127" s="36">
+        <v>44137.145833333336</v>
+      </c>
+      <c r="D127" s="123">
+        <v>0.02</v>
+      </c>
+      <c r="E127" s="126">
+        <v>54.6</v>
+      </c>
+      <c r="F127" s="114">
+        <v>307</v>
+      </c>
+      <c r="G127" s="13">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H127" s="13">
+        <v>-2.1</v>
+      </c>
+      <c r="I127" s="13">
+        <f t="shared" ref="I127" si="208">-LOG((1/(G127^2))*(2.511^(-H127)))/LOG(2.511)</f>
+        <v>4.396755056942248</v>
+      </c>
+      <c r="J127" s="121" t="s">
+        <v>435</v>
+      </c>
+      <c r="K127" s="121"/>
+      <c r="L127" s="121"/>
+      <c r="M127" s="13">
+        <v>48</v>
+      </c>
+      <c r="N127" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O127" s="5">
+        <v>0</v>
+      </c>
+      <c r="P127" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q127" s="22"/>
+      <c r="R127" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S127" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T127" s="256">
+        <f t="shared" ref="T127" si="209">1/SIN(RADIANS(M127+244/(165+47*M127^1.1)))</f>
+        <v>1.3441558434238583</v>
+      </c>
+      <c r="U127" s="114">
+        <f t="shared" ref="U127" si="210">DEGREES(ASIN(SIN(RADIANS(F127))*SIN(RADIANS(25.19))))</f>
+        <v>-19.871776787349532</v>
+      </c>
+      <c r="V127" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W127" s="26">
+        <f t="shared" ref="W127" si="211">668.5921*MOD((C127-Z$1),686.9726)/686.9726</f>
+        <v>573.84431181729769</v>
+      </c>
+      <c r="X127" s="26">
+        <f t="shared" ref="X127" si="212">(S127/(G127/2))*T127/(IF(ISBLANK(N127),0.5,N127))</f>
+        <v>7.0922795758545279E-2</v>
+      </c>
+      <c r="Y127" s="26">
+        <f t="shared" ref="Y127" si="213">0.1/X127</f>
+        <v>1.4099838977082526</v>
+      </c>
+    </row>
+    <row r="128" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="22"/>
+      <c r="C128" s="36">
+        <v>44138.166666666664</v>
+      </c>
+      <c r="D128" s="123">
+        <v>0.02</v>
+      </c>
+      <c r="E128" s="126">
+        <v>53</v>
+      </c>
+      <c r="F128" s="114">
+        <v>308</v>
+      </c>
+      <c r="G128" s="13">
+        <v>19.7</v>
+      </c>
+      <c r="H128" s="13">
+        <v>-2.1</v>
+      </c>
+      <c r="I128" s="13">
+        <f t="shared" ref="I128" si="214">-LOG((1/(G128^2))*(2.511^(-H128)))/LOG(2.511)</f>
+        <v>4.3748123968745976</v>
+      </c>
+      <c r="J128" s="121" t="s">
+        <v>435</v>
+      </c>
+      <c r="K128" s="121"/>
+      <c r="L128" s="121"/>
+      <c r="M128" s="13">
+        <v>52</v>
+      </c>
+      <c r="N128" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O128" s="5">
+        <v>0</v>
+      </c>
+      <c r="P128" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q128" s="22"/>
+      <c r="R128" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S128" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T128" s="256">
+        <f t="shared" ref="T128" si="215">1/SIN(RADIANS(M128+244/(165+47*M128^1.1)))</f>
+        <v>1.2679069016723665</v>
+      </c>
+      <c r="U128" s="114">
+        <f t="shared" ref="U128" si="216">DEGREES(ASIN(SIN(RADIANS(F128))*SIN(RADIANS(25.19))))</f>
+        <v>-19.596511487075084</v>
+      </c>
+      <c r="V128" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W128" s="26">
+        <f t="shared" ref="W128" si="217">668.5921*MOD((C128-Z$1),686.9726)/686.9726</f>
+        <v>574.83783194034197</v>
+      </c>
+      <c r="X128" s="26">
+        <f t="shared" ref="X128" si="218">(S128/(G128/2))*T128/(IF(ISBLANK(N128),0.5,N128))</f>
+        <v>6.757879425157283E-2</v>
+      </c>
+      <c r="Y128" s="26">
+        <f t="shared" ref="Y128" si="219">0.1/X128</f>
+        <v>1.4797541315657996</v>
+      </c>
+    </row>
+    <row r="129" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="22"/>
+      <c r="C129" s="36">
+        <v>44141.15625</v>
+      </c>
+      <c r="D129" s="123">
+        <v>0.03</v>
+      </c>
+      <c r="E129" s="126">
+        <v>22.3</v>
+      </c>
+      <c r="F129" s="114">
+        <v>310</v>
+      </c>
+      <c r="G129" s="13">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="H129" s="13">
+        <v>-2</v>
+      </c>
+      <c r="I129" s="13">
+        <f t="shared" ref="I129" si="220">-LOG((1/(G129^2))*(2.511^(-H129)))/LOG(2.511)</f>
+        <v>4.4076223538567385</v>
+      </c>
+      <c r="J129" s="121" t="s">
+        <v>435</v>
+      </c>
+      <c r="K129" s="121"/>
+      <c r="L129" s="121"/>
+      <c r="M129" s="13">
+        <v>52</v>
+      </c>
+      <c r="N129" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O129" s="5">
+        <v>0</v>
+      </c>
+      <c r="P129" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q129" s="22"/>
+      <c r="R129" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S129" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T129" s="256">
+        <f t="shared" ref="T129" si="221">1/SIN(RADIANS(M129+244/(165+47*M129^1.1)))</f>
+        <v>1.2679069016723665</v>
+      </c>
+      <c r="U129" s="114">
+        <f t="shared" ref="U129" si="222">DEGREES(ASIN(SIN(RADIANS(F129))*SIN(RADIANS(25.19))))</f>
+        <v>-19.028890741463773</v>
+      </c>
+      <c r="V129" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W129" s="26">
+        <f t="shared" ref="W129" si="223">668.5921*MOD((C129-Z$1),686.9726)/686.9726</f>
+        <v>577.74742658641662</v>
+      </c>
+      <c r="X129" s="26">
+        <f t="shared" ref="X129" si="224">(S129/(G129/2))*T129/(IF(ISBLANK(N129),0.5,N129))</f>
+        <v>6.9701688311831655E-2</v>
+      </c>
+      <c r="Y129" s="26">
+        <f t="shared" ref="Y129" si="225">0.1/X129</f>
+        <v>1.4346854778125266</v>
+      </c>
+    </row>
+    <row r="130" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="22"/>
+      <c r="C130" s="36">
+        <v>44152.125</v>
+      </c>
+      <c r="D130" s="123">
+        <v>0.05</v>
+      </c>
+      <c r="E130" s="126">
+        <v>271.3</v>
+      </c>
+      <c r="F130" s="114">
+        <v>316</v>
+      </c>
+      <c r="G130" s="13">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="H130" s="13">
+        <v>-1.6</v>
+      </c>
+      <c r="I130" s="13">
+        <f t="shared" ref="I130" si="226">-LOG((1/(G130^2))*(2.511^(-H130)))/LOG(2.511)</f>
+        <v>4.5673439905327262</v>
+      </c>
+      <c r="J130" s="121" t="s">
+        <v>435</v>
+      </c>
+      <c r="K130" s="121"/>
+      <c r="L130" s="121"/>
+      <c r="M130" s="13">
+        <v>52</v>
+      </c>
+      <c r="N130" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O130" s="5">
+        <v>0</v>
+      </c>
+      <c r="P130" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q130" s="22"/>
+      <c r="R130" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S130" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T130" s="256">
+        <f t="shared" ref="T130" si="227">1/SIN(RADIANS(M130+244/(165+47*M130^1.1)))</f>
+        <v>1.2679069016723665</v>
+      </c>
+      <c r="U130" s="114">
+        <f t="shared" ref="U130" si="228">DEGREES(ASIN(SIN(RADIANS(F130))*SIN(RADIANS(25.19))))</f>
+        <v>-17.197204585190082</v>
+      </c>
+      <c r="V130" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W130" s="26">
+        <f t="shared" ref="W130" si="229">668.5921*MOD((C130-Z$1),686.9726)/686.9726</f>
+        <v>588.42269892897434</v>
+      </c>
+      <c r="X130" s="26">
+        <f t="shared" ref="X130" si="230">(S130/(G130/2))*T130/(IF(ISBLANK(N130),0.5,N130))</f>
+        <v>7.7853932558829511E-2</v>
+      </c>
+      <c r="Y130" s="26">
+        <f t="shared" ref="Y130" si="231">0.1/X130</f>
+        <v>1.2844566319682831</v>
+      </c>
+    </row>
+    <row r="131" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="22"/>
+      <c r="C131" s="36">
+        <v>44153.21875</v>
+      </c>
+      <c r="D131" s="123">
+        <v>0.05</v>
+      </c>
+      <c r="E131" s="126">
+        <v>295</v>
+      </c>
+      <c r="F131" s="114">
+        <v>317</v>
+      </c>
+      <c r="G131" s="13">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H131" s="13">
+        <v>-1.6</v>
+      </c>
+      <c r="I131" s="13">
+        <f t="shared" ref="I131" si="232">-LOG((1/(G131^2))*(2.511^(-H131)))/LOG(2.511)</f>
+        <v>4.5417871678002673</v>
+      </c>
+      <c r="J131" s="121" t="s">
+        <v>435</v>
+      </c>
+      <c r="K131" s="121"/>
+      <c r="L131" s="121"/>
+      <c r="M131" s="13">
+        <v>52</v>
+      </c>
+      <c r="N131" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O131" s="5">
+        <v>0</v>
+      </c>
+      <c r="P131" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q131" s="22"/>
+      <c r="R131" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S131" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T131" s="256">
+        <f t="shared" ref="T131" si="233">1/SIN(RADIANS(M131+244/(165+47*M131^1.1)))</f>
+        <v>1.2679069016723665</v>
+      </c>
+      <c r="U131" s="114">
+        <f t="shared" ref="U131" si="234">DEGREES(ASIN(SIN(RADIANS(F131))*SIN(RADIANS(25.19))))</f>
+        <v>-16.874305122260981</v>
+      </c>
+      <c r="V131" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W131" s="26">
+        <f t="shared" ref="W131" si="235">668.5921*MOD((C131-Z$1),686.9726)/686.9726</f>
+        <v>589.4871847750984</v>
+      </c>
+      <c r="X131" s="26">
+        <f t="shared" ref="X131" si="236">(S131/(G131/2))*T131/(IF(ISBLANK(N131),0.5,N131))</f>
+        <v>7.8775280873135206E-2</v>
+      </c>
+      <c r="Y131" s="26">
+        <f t="shared" ref="Y131" si="237">0.1/X131</f>
+        <v>1.2694337473838584</v>
+      </c>
+    </row>
+    <row r="132" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="22"/>
+      <c r="C132" s="36">
+        <v>44164.114583333336</v>
+      </c>
+      <c r="D132" s="123">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E132" s="126">
+        <v>156.6</v>
+      </c>
+      <c r="F132" s="114">
+        <v>323</v>
+      </c>
+      <c r="G132" s="13">
+        <v>14.9</v>
+      </c>
+      <c r="H132" s="13">
+        <v>-1.2</v>
+      </c>
+      <c r="I132" s="13">
+        <f t="shared" ref="I132" si="238">-LOG((1/(G132^2))*(2.511^(-H132)))/LOG(2.511)</f>
+        <v>4.6681801355940395</v>
+      </c>
+      <c r="J132" s="121" t="s">
+        <v>435</v>
+      </c>
+      <c r="K132" s="121"/>
+      <c r="L132" s="121"/>
+      <c r="M132" s="13">
+        <v>55</v>
+      </c>
+      <c r="N132" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O132" s="5">
+        <v>0</v>
+      </c>
+      <c r="P132" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q132" s="22"/>
+      <c r="R132" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S132" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T132" s="256">
+        <f t="shared" ref="T132" si="239">1/SIN(RADIANS(M132+244/(165+47*M132^1.1)))</f>
+        <v>1.2198713542670481</v>
+      </c>
+      <c r="U132" s="114">
+        <f t="shared" ref="U132" si="240">DEGREES(ASIN(SIN(RADIANS(F132))*SIN(RADIANS(25.19))))</f>
+        <v>-14.841461952952889</v>
+      </c>
+      <c r="V132" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W132" s="26">
+        <f t="shared" ref="W132" si="241">668.5921*MOD((C132-Z$1),686.9726)/686.9726</f>
+        <v>600.0914913945835</v>
+      </c>
+      <c r="X132" s="26">
+        <f t="shared" ref="X132" si="242">(S132/(G132/2))*T132/(IF(ISBLANK(N132),0.5,N132))</f>
+        <v>8.5964088723516796E-2</v>
+      </c>
+      <c r="Y132" s="26">
+        <f t="shared" ref="Y132" si="243">0.1/X132</f>
+        <v>1.1632764504911628</v>
+      </c>
+    </row>
+    <row r="133" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="22"/>
+      <c r="C133" s="36">
+        <v>44172.145833333336</v>
+      </c>
+      <c r="D133" s="123">
+        <v>0.09</v>
+      </c>
+      <c r="E133" s="126">
+        <v>92.5</v>
+      </c>
+      <c r="F133" s="114">
+        <v>327</v>
+      </c>
+      <c r="G133" s="13">
+        <v>13.6</v>
+      </c>
+      <c r="H133" s="13">
+        <v>-0.9</v>
+      </c>
+      <c r="I133" s="13">
+        <f t="shared" ref="I133" si="244">-LOG((1/(G133^2))*(2.511^(-H133)))/LOG(2.511)</f>
+        <v>4.7698673383070345</v>
+      </c>
+      <c r="J133" s="121" t="s">
+        <v>435</v>
+      </c>
+      <c r="K133" s="121"/>
+      <c r="L133" s="121"/>
+      <c r="M133" s="13">
+        <v>57</v>
+      </c>
+      <c r="N133" s="267">
+        <v>0.8</v>
+      </c>
+      <c r="O133" s="5">
+        <v>0</v>
+      </c>
+      <c r="P133" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q133" s="22"/>
+      <c r="R133" s="6">
+        <v>44053</v>
+      </c>
+      <c r="S133" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="T133" s="256">
+        <f t="shared" ref="T133" si="245">1/SIN(RADIANS(M133+244/(165+47*M133^1.1)))</f>
+        <v>1.1915753236973983</v>
+      </c>
+      <c r="U133" s="114">
+        <f t="shared" ref="U133" si="246">DEGREES(ASIN(SIN(RADIANS(F133))*SIN(RADIANS(25.19))))</f>
+        <v>-13.403657961356764</v>
+      </c>
+      <c r="V133" s="114">
+        <v>22.22</v>
+      </c>
+      <c r="W133" s="26">
+        <f t="shared" ref="W133" si="247">668.5921*MOD((C133-Z$1),686.9726)/686.9726</f>
+        <v>607.90785889326548</v>
+      </c>
+      <c r="X133" s="26">
+        <f t="shared" ref="X133" si="248">(S133/(G133/2))*T133/(IF(ISBLANK(N133),0.5,N133))</f>
+        <v>9.1996624256049125E-2</v>
+      </c>
+      <c r="Y133" s="26">
+        <f t="shared" ref="Y133" si="249">0.1/X133</f>
+        <v>1.086996406755921</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AA92" xr:uid="{00000000-0009-0000-0000-000004000000}"/>

</xml_diff>